<commit_message>
Save 68bus test case
</commit_message>
<xml_diff>
--- a/Nature_NETS_NYPS_68Bus_HybridSGIBR.xlsx
+++ b/Nature_NETS_NYPS_68Bus_HybridSGIBR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yg934\GitHub\Power-Communication-Isomorphism\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E989082-ABF1-48F9-841E-CF223A5C5226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8699DE4-35B6-4A46-80A7-12BE721B8389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="12852" windowWidth="19416" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -239,20 +239,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.00_ "/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -261,7 +261,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -269,7 +269,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -277,7 +277,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -285,13 +285,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -304,7 +304,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -343,27 +343,27 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -648,23 +648,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" customWidth="1"/>
+    <col min="10" max="10" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -702,7 +702,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -740,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -816,7 +816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -854,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="6">
-        <v>-1</v>
+        <v>-0.01</v>
       </c>
       <c r="F7" s="8">
         <v>0</v>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A55" s="6">
         <v>53</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A56" s="6">
         <v>54</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A57" s="6">
         <v>55</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A58" s="6">
         <v>56</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A59" s="6">
         <v>57</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>58</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>59</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>60</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3297,34 +3297,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.796875" customWidth="1"/>
+    <col min="2" max="2" width="29.53125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.109375" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" customWidth="1"/>
+    <col min="5" max="5" width="12.46484375" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" customWidth="1"/>
+    <col min="7" max="7" width="13.796875" customWidth="1"/>
+    <col min="8" max="8" width="15.1328125" customWidth="1"/>
+    <col min="9" max="9" width="18.796875" customWidth="1"/>
+    <col min="10" max="10" width="18.53125" customWidth="1"/>
+    <col min="11" max="11" width="17.1328125" customWidth="1"/>
+    <col min="12" max="12" width="17.86328125" customWidth="1"/>
+    <col min="13" max="13" width="14.46484375" customWidth="1"/>
+    <col min="14" max="14" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -3343,10 +3343,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="12">
-        <v>10</v>
+        <v>1000000000</v>
       </c>
       <c r="D3" s="12">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="E3" s="12">
         <v>1.0000000000000001E-5</v>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -3380,7 +3380,7 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="8">
         <v>15</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="8">
         <v>18</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="8">
         <v>19</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="8">
         <v>28</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="8">
         <v>29</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="6">
         <v>31</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="6">
         <v>32</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="6">
         <v>33</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="6">
         <v>34</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="6">
         <v>35</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="6">
         <v>36</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="6">
         <v>37</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="6">
         <v>38</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="6">
         <v>39</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="6">
         <v>40</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="6">
         <v>41</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="6">
         <v>42</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="6">
         <v>43</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="6">
         <v>44</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="6">
         <v>45</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="6">
         <v>46</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" s="6">
         <v>47</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" s="6">
         <v>48</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" s="6">
         <v>49</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" s="6">
         <v>50</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" s="6">
         <v>51</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" s="6">
         <v>52</v>
       </c>
@@ -4451,7 +4451,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" s="6">
         <v>53</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" s="6">
         <v>54</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" s="6">
         <v>55</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" s="6">
         <v>56</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" s="6">
         <v>57</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4667,7 +4667,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4808,33 +4808,33 @@
       <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="10">
         <v>16</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>2</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>3</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>4</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>5</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>1.0089999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>6</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>7</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>8</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>9</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>1.0249999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>10</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>11</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>12</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>13</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>14</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>15</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="10">
         <v>1</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>17</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>18</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>18</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>19</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>20</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>21</v>
       </c>
@@ -5363,7 +5363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>22</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>23</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>24</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>24</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>25</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>26</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>27</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>27</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>28</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>29</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A38">
         <v>29</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39">
         <v>30</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40">
         <v>30</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>31</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>31</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>32</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>33</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>34</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46">
         <v>34</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>0.94599999999999995</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47">
         <v>36</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A48">
         <v>36</v>
       </c>
@@ -5846,7 +5846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>37</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>38</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A51">
         <v>38</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A52">
         <v>40</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A53">
         <v>40</v>
       </c>
@@ -5961,7 +5961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>41</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>42</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A56">
         <v>43</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>44</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>44</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A59">
         <v>45</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A60">
         <v>45</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A61">
         <v>45</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A62">
         <v>46</v>
       </c>
@@ -6168,7 +6168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>47</v>
       </c>
@@ -6191,7 +6191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>48</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A65">
         <v>49</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A66">
         <v>51</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A67">
         <v>51</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A68">
         <v>52</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A69">
         <v>52</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A70">
         <v>54</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A71">
         <v>55</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>56</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>57</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A74">
         <v>58</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A75">
         <v>59</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A76">
         <v>60</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>60</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>61</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A79">
         <v>63</v>
       </c>
@@ -6559,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A80">
         <v>63</v>
       </c>
@@ -6582,7 +6582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>63</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A82">
         <v>65</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>65</v>
       </c>
@@ -6651,7 +6651,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>66</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A85">
         <v>66</v>
       </c>
@@ -6697,7 +6697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>67</v>
       </c>
@@ -6720,7 +6720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A87">
         <v>68</v>
       </c>
@@ -6743,7 +6743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>27</v>
       </c>
@@ -6781,18 +6781,18 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -6830,20 +6830,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -6852,7 +6852,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -6888,20 +6888,20 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="30.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
@@ -6910,7 +6910,7 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -6982,12 +6982,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>44</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>